<commit_message>
reduced test scenario to 50 timesteps
</commit_message>
<xml_diff>
--- a/data/TestScenario/input_data/scenario_settings.xlsx
+++ b/data/TestScenario/input_data/scenario_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70b0e526faaa1b23/Dokumente/Alles zum Studium/Master/Masterarbeit/Leelo/data/TestScenario/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F53D9131-8A1D-4626-A9A9-63BAC14608FC}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2525993-9B3A-4D29-A60A-44D1C7007EA3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="876" yWindow="1020" windowWidth="20736" windowHeight="10752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="A1:AL26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +678,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>8760</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>1</v>

</xml_diff>